<commit_message>
import expost siswa "waka"
</commit_message>
<xml_diff>
--- a/files/sample_siswa.xlsx
+++ b/files/sample_siswa.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmadhanafi\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="siswa" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>no</t>
   </si>
@@ -47,35 +42,44 @@
     <t>jk</t>
   </si>
   <si>
-    <t>Ahmad Hanafi</t>
-  </si>
-  <si>
     <t>12 MM2</t>
   </si>
   <si>
     <t>L</t>
   </si>
   <si>
-    <t>Siti Maryam</t>
-  </si>
-  <si>
-    <t>11 AP1</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Abdul Qodir</t>
-  </si>
-  <si>
-    <t>10 AK4</t>
+    <t>tempat</t>
+  </si>
+  <si>
+    <t>tanggal_lahir</t>
+  </si>
+  <si>
+    <t>alamat_lengkap</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>nomer_telp</t>
+  </si>
+  <si>
+    <t>temanggung</t>
+  </si>
+  <si>
+    <t>sabrang@gmail.com</t>
+  </si>
+  <si>
+    <t>Sabrang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,9 +97,25 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -116,22 +136,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,9 +454,11 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -447,8 +480,23 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -458,67 +506,39 @@
       <c r="C2" s="3">
         <v>9983782434</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E2" s="2">
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>141510600</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9082018888</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>141510900</v>
-      </c>
-      <c r="C4" s="2">
-        <v>9082012192</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
+      <c r="I2" s="6">
+        <v>38334</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2">
+        <v>89509518038</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>